<commit_message>
fix unit most of unit tests
</commit_message>
<xml_diff>
--- a/ExampleFiles/Gantt/team.xlsx
+++ b/ExampleFiles/Gantt/team.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC07E3B-4D57-4327-99B5-3894F2460B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D69C7-C78A-40B1-9766-BD77ACCEE75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamsSimple" sheetId="1" r:id="rId1"/>
     <sheet name="TeamsMultiple" sheetId="2" r:id="rId2"/>
+    <sheet name="TeamsSimpleVacation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>Team Name</t>
   </si>
@@ -71,6 +72,12 @@
   </si>
   <si>
     <t>Developer Id</t>
+  </si>
+  <si>
+    <t>2025-03-10;2025-03-15|2025-05-10;2025-05-15|2025-05-19;2025-05-19</t>
+  </si>
+  <si>
+    <t>2025-03-10;2025-03-15|2025-05-10;2025-05-15|</t>
   </si>
 </sst>
 </file>
@@ -156,6 +163,21 @@
     <tableColumn id="2" xr3:uid="{867737E7-AFEF-412E-A075-817ABE763996}" name="Developer Name"/>
     <tableColumn id="3" xr3:uid="{636A2CBF-D0B7-488C-928E-CBC6E647B7D9}" name="Developer Vacation Date Intervals"/>
     <tableColumn id="4" xr3:uid="{985D3BC6-6C0E-43A5-A32C-1C190F9E8023}" name="Daily Work Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D25E0757-6E1A-4BCE-98E5-25F4A1E42105}" name="Table14" displayName="Table14" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{5156F39C-A57D-49CD-8981-173D65261D30}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{1BFD1882-3482-4B20-B20B-55E1E4B9AD3A}" name="Team ID"/>
+    <tableColumn id="1" xr3:uid="{842B82D1-73CE-47B7-93C4-28147EB6CBB8}" name="Team Name"/>
+    <tableColumn id="5" xr3:uid="{E5B279B2-A853-429B-84E9-2F3F0844BF44}" name="Developer Id"/>
+    <tableColumn id="2" xr3:uid="{4679F434-B323-45FB-94E3-02BE0961DD76}" name="Developer Name"/>
+    <tableColumn id="3" xr3:uid="{973910BB-0B46-41AC-9E98-CB9EE6F85968}" name="Developer Vacation Date Intervals"/>
+    <tableColumn id="4" xr3:uid="{9A768427-56AB-41F5-AB6D-221C181C4A60}" name="Daily Work Hours"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,7 +449,129 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1A7527-178D-4A07-9D68-FBCE235309E3}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,10 +641,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -517,10 +661,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -536,7 +680,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -544,12 +687,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1A7527-178D-4A07-9D68-FBCE235309E3}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8AA253-47B4-46EA-A3A5-685EE8FE0B92}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,7 +700,7 @@
     <col min="1" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -594,7 +737,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -614,15 +757,15 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -639,10 +782,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>4</v>

</xml_diff>